<commit_message>
f and p calculated as single blocks
</commit_message>
<xml_diff>
--- a/footprints.xlsx
+++ b/footprints.xlsx
@@ -552,13 +552,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>43.59163834561823</v>
+        <v>43.59163834560552</v>
       </c>
       <c r="C2">
-        <v>33.6870015388355</v>
+        <v>33.68700153881799</v>
       </c>
       <c r="D2">
-        <v>44.54200221933364</v>
+        <v>44.54200221933983</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -566,13 +566,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>62.22037985068946</v>
+        <v>62.22037985068194</v>
       </c>
       <c r="C3">
-        <v>53.71445327132803</v>
+        <v>53.71445327132621</v>
       </c>
       <c r="D3">
-        <v>55.83895923802991</v>
+        <v>55.83895923802758</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -580,13 +580,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>34.20132479538303</v>
+        <v>34.2013247953663</v>
       </c>
       <c r="C4">
-        <v>25.91558036587688</v>
+        <v>25.91558036586404</v>
       </c>
       <c r="D4">
-        <v>33.93924910334591</v>
+        <v>33.93924910334658</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -594,13 +594,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>65.31566886823093</v>
+        <v>65.31566886820625</v>
       </c>
       <c r="C5">
-        <v>47.48946758417029</v>
+        <v>47.48946758418124</v>
       </c>
       <c r="D5">
-        <v>57.72684498040659</v>
+        <v>57.72684498059444</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -608,13 +608,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>21.59714398111019</v>
+        <v>21.59714398111175</v>
       </c>
       <c r="C6">
-        <v>20.82788481004459</v>
+        <v>20.82788481004951</v>
       </c>
       <c r="D6">
-        <v>21.60414120775898</v>
+        <v>21.60414120774838</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -622,13 +622,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>45.44557868891953</v>
+        <v>45.445578688912</v>
       </c>
       <c r="C7">
-        <v>38.06994933676467</v>
+        <v>38.0699493367692</v>
       </c>
       <c r="D7">
-        <v>43.57323984926443</v>
+        <v>43.57323984925853</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -636,13 +636,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>31.17745687962519</v>
+        <v>31.17745687962574</v>
       </c>
       <c r="C8">
-        <v>33.412105558346</v>
+        <v>33.41210555835896</v>
       </c>
       <c r="D8">
-        <v>32.96685159550108</v>
+        <v>32.9668515955231</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -650,13 +650,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>83.12911655546704</v>
+        <v>83.12911655545818</v>
       </c>
       <c r="C9">
-        <v>80.39923753049139</v>
+        <v>80.39923753048055</v>
       </c>
       <c r="D9">
-        <v>85.10865184518721</v>
+        <v>85.10865184518886</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -664,13 +664,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>70.58933020047705</v>
+        <v>70.5893302004559</v>
       </c>
       <c r="C10">
-        <v>75.37717886312569</v>
+        <v>75.37717886332202</v>
       </c>
       <c r="D10">
-        <v>92.55426945182941</v>
+        <v>92.55426945210493</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -678,13 +678,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>84.36759528240096</v>
+        <v>84.36759528236909</v>
       </c>
       <c r="C11">
-        <v>72.35493180643803</v>
+        <v>72.3549318065689</v>
       </c>
       <c r="D11">
-        <v>79.32357377917563</v>
+        <v>79.32357377937842</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -692,13 +692,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>52.9471424041587</v>
+        <v>52.94714240415751</v>
       </c>
       <c r="C12">
-        <v>40.07183878366896</v>
+        <v>40.07183878365237</v>
       </c>
       <c r="D12">
-        <v>50.0983782087788</v>
+        <v>50.09837820878275</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -706,13 +706,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>41.35328616527512</v>
+        <v>41.35328616527343</v>
       </c>
       <c r="C13">
-        <v>49.24801083412337</v>
+        <v>49.24801083438491</v>
       </c>
       <c r="D13">
-        <v>50.81675406893512</v>
+        <v>50.81675406921465</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -720,13 +720,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>56.91502147563941</v>
+        <v>56.91502147567003</v>
       </c>
       <c r="C14">
-        <v>52.6773661946839</v>
+        <v>52.67736619467398</v>
       </c>
       <c r="D14">
-        <v>58.63790063070515</v>
+        <v>58.63790063068734</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -734,13 +734,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>27.39198973868829</v>
+        <v>27.39198973865176</v>
       </c>
       <c r="C15">
-        <v>21.61905002091946</v>
+        <v>21.61905002090086</v>
       </c>
       <c r="D15">
-        <v>29.57902700890774</v>
+        <v>29.5790270089253</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -748,13 +748,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>42.30873323253078</v>
+        <v>42.30873323249113</v>
       </c>
       <c r="C16">
-        <v>36.76159686313855</v>
+        <v>36.76159686315574</v>
       </c>
       <c r="D16">
-        <v>39.92508584652658</v>
+        <v>39.92508584653299</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -762,13 +762,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>43.09481853461209</v>
+        <v>43.09481853462169</v>
       </c>
       <c r="C17">
-        <v>44.15226414604586</v>
+        <v>44.15226414608404</v>
       </c>
       <c r="D17">
-        <v>47.76986446966103</v>
+        <v>47.76986446966652</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -776,13 +776,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>38.85190256495495</v>
+        <v>38.85190256496871</v>
       </c>
       <c r="C18">
-        <v>29.87148193617369</v>
+        <v>29.87148193613448</v>
       </c>
       <c r="D18">
-        <v>38.9534869948864</v>
+        <v>38.95348699490175</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -790,13 +790,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>67.58123710625787</v>
+        <v>67.58123710626089</v>
       </c>
       <c r="C19">
-        <v>53.54946630543632</v>
+        <v>53.54946630544881</v>
       </c>
       <c r="D19">
-        <v>61.99429322278958</v>
+        <v>61.99429322276653</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -804,13 +804,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>67.31178111553862</v>
+        <v>67.31178111556743</v>
       </c>
       <c r="C20">
-        <v>68.28112211594342</v>
+        <v>68.28112211596651</v>
       </c>
       <c r="D20">
-        <v>92.44452950883247</v>
+        <v>92.44452950893114</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -818,13 +818,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>46.84771038666729</v>
+        <v>46.84771038668232</v>
       </c>
       <c r="C21">
-        <v>35.31279684452878</v>
+        <v>35.31279684456659</v>
       </c>
       <c r="D21">
-        <v>45.20903183657334</v>
+        <v>45.20903183676453</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -832,13 +832,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>93.02344139758833</v>
+        <v>93.02344139748631</v>
       </c>
       <c r="C22">
-        <v>77.46599869077509</v>
+        <v>77.46599869070562</v>
       </c>
       <c r="D22">
-        <v>85.68356792573199</v>
+        <v>85.68356792565694</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -846,13 +846,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>38.26509245799652</v>
+        <v>38.26509245801047</v>
       </c>
       <c r="C23">
-        <v>41.88985110477778</v>
+        <v>41.88985110486191</v>
       </c>
       <c r="D23">
-        <v>44.34731748376406</v>
+        <v>44.34731748394536</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -860,13 +860,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>100.4315316324279</v>
+        <v>100.4315316324218</v>
       </c>
       <c r="C24">
-        <v>72.19343092617888</v>
+        <v>72.19343092623272</v>
       </c>
       <c r="D24">
-        <v>84.08847786107405</v>
+        <v>84.08847786114049</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -874,13 +874,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>67.12230080674723</v>
+        <v>67.12230080674995</v>
       </c>
       <c r="C25">
-        <v>49.09541830964711</v>
+        <v>49.09541830964331</v>
       </c>
       <c r="D25">
-        <v>61.46692305830008</v>
+        <v>61.46692305829972</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -888,13 +888,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>71.00923507759074</v>
+        <v>71.00923507755903</v>
       </c>
       <c r="C26">
-        <v>53.08705790241792</v>
+        <v>53.08705790242317</v>
       </c>
       <c r="D26">
-        <v>63.07808737301927</v>
+        <v>63.07808737303417</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -902,13 +902,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>101.0371283201483</v>
+        <v>101.0371283200779</v>
       </c>
       <c r="C27">
-        <v>114.5366229150995</v>
+        <v>114.5366229150276</v>
       </c>
       <c r="D27">
-        <v>105.4896392664579</v>
+        <v>105.4896392664067</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -916,13 +916,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>56.89450191496697</v>
+        <v>56.89450191495735</v>
       </c>
       <c r="C28">
-        <v>52.12475460088764</v>
+        <v>52.12475460087984</v>
       </c>
       <c r="D28">
-        <v>61.76496674164599</v>
+        <v>61.76496674166857</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -930,13 +930,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>41.98678072011969</v>
+        <v>41.98678072010747</v>
       </c>
       <c r="C29">
-        <v>42.45393739373015</v>
+        <v>42.45393739373337</v>
       </c>
       <c r="D29">
-        <v>43.41874764961742</v>
+        <v>43.41874764962718</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -944,13 +944,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>53.95826673110527</v>
+        <v>53.95826673108189</v>
       </c>
       <c r="C30">
-        <v>52.06885433977128</v>
+        <v>52.06885433975418</v>
       </c>
       <c r="D30">
-        <v>61.41468415403919</v>
+        <v>61.41468415405209</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -958,13 +958,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>20.30742737852042</v>
+        <v>20.30742737852825</v>
       </c>
       <c r="C31">
-        <v>33.46955956596231</v>
+        <v>33.4695595661413</v>
       </c>
       <c r="D31">
-        <v>34.2299490534669</v>
+        <v>34.22994905351453</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -972,13 +972,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>54.31086965151725</v>
+        <v>54.31086965150902</v>
       </c>
       <c r="C32">
-        <v>39.37121963596453</v>
+        <v>39.37121963589789</v>
       </c>
       <c r="D32">
-        <v>48.5531231218349</v>
+        <v>48.55312312180118</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -986,13 +986,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>55.69450903470714</v>
+        <v>55.69450903469122</v>
       </c>
       <c r="C33">
-        <v>41.46270304069485</v>
+        <v>41.46270304064971</v>
       </c>
       <c r="D33">
-        <v>51.4731752877094</v>
+        <v>51.47317528767589</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1000,13 +1000,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>22.28740813010213</v>
+        <v>22.28740813015425</v>
       </c>
       <c r="C34">
-        <v>21.11263260327238</v>
+        <v>21.11263260325514</v>
       </c>
       <c r="D34">
-        <v>24.11313449956385</v>
+        <v>24.11313449957503</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1014,13 +1014,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>88.20107318144332</v>
+        <v>88.20107318147582</v>
       </c>
       <c r="C35">
-        <v>86.11679745901905</v>
+        <v>86.11679745904493</v>
       </c>
       <c r="D35">
-        <v>87.37860948613448</v>
+        <v>87.37860948632166</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1028,13 +1028,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>22.03554878838386</v>
+        <v>22.03554878836278</v>
       </c>
       <c r="C36">
-        <v>17.36219749247004</v>
+        <v>17.36219749244167</v>
       </c>
       <c r="D36">
-        <v>23.42819494356797</v>
+        <v>23.42819494355437</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1042,13 +1042,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>74.10347248729077</v>
+        <v>74.10347248726494</v>
       </c>
       <c r="C37">
-        <v>53.70391856764511</v>
+        <v>53.70391856760934</v>
       </c>
       <c r="D37">
-        <v>68.24642134765571</v>
+        <v>68.2464213479399</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1056,13 +1056,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>79.11076297335535</v>
+        <v>79.11076297330058</v>
       </c>
       <c r="C38">
-        <v>69.52782998777175</v>
+        <v>69.5278299877299</v>
       </c>
       <c r="D38">
-        <v>75.79658193181858</v>
+        <v>75.79658193176628</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1070,13 +1070,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>25.29035203061651</v>
+        <v>25.29035203060509</v>
       </c>
       <c r="C39">
-        <v>19.68737734299174</v>
+        <v>19.68737734295507</v>
       </c>
       <c r="D39">
-        <v>26.44260115650944</v>
+        <v>26.44260115651526</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1084,13 +1084,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>63.02333411552829</v>
+        <v>63.02333411551123</v>
       </c>
       <c r="C40">
-        <v>59.33478841632653</v>
+        <v>59.33478841644541</v>
       </c>
       <c r="D40">
-        <v>63.3861344808397</v>
+        <v>63.38613448100399</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1098,13 +1098,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>79.787425980314</v>
+        <v>79.78742598024895</v>
       </c>
       <c r="C41">
-        <v>69.89490723315178</v>
+        <v>69.89490723324111</v>
       </c>
       <c r="D41">
-        <v>76.26518976156255</v>
+        <v>76.26518976175447</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1112,13 +1112,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>68.25160556302365</v>
+        <v>68.25160556304937</v>
       </c>
       <c r="C42">
-        <v>67.58436042333376</v>
+        <v>67.58436042322373</v>
       </c>
       <c r="D42">
-        <v>65.41446644525726</v>
+        <v>65.41446644522435</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1126,13 +1126,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>58.85049838789674</v>
+        <v>58.85049838786862</v>
       </c>
       <c r="C43">
-        <v>43.56834465142425</v>
+        <v>43.56834465144687</v>
       </c>
       <c r="D43">
-        <v>53.34876334768916</v>
+        <v>53.34876334769473</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1140,13 +1140,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>87.9634191720352</v>
+        <v>87.96341917200768</v>
       </c>
       <c r="C44">
-        <v>64.70282614070773</v>
+        <v>64.70282614072794</v>
       </c>
       <c r="D44">
-        <v>80.07231657602014</v>
+        <v>80.07231657604686</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1154,13 +1154,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>108.2144218458915</v>
+        <v>108.2144218459599</v>
       </c>
       <c r="C45">
-        <v>111.3209353718248</v>
+        <v>111.3209353718479</v>
       </c>
       <c r="D45">
-        <v>104.0616694795949</v>
+        <v>104.0616694796631</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1168,13 +1168,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>55.51040738154471</v>
+        <v>55.51040738164549</v>
       </c>
       <c r="C46">
-        <v>51.95429109544557</v>
+        <v>51.95429109556157</v>
       </c>
       <c r="D46">
-        <v>51.59090314784817</v>
+        <v>51.59090314791123</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1182,13 +1182,13 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>44.86274329919177</v>
+        <v>44.86274329918177</v>
       </c>
       <c r="C47">
-        <v>42.11541492422086</v>
+        <v>42.11541492421686</v>
       </c>
       <c r="D47">
-        <v>46.98745263017619</v>
+        <v>46.9874526302014</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1196,13 +1196,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>69.22181872944999</v>
+        <v>69.22181872943298</v>
       </c>
       <c r="C48">
-        <v>50.62751318870081</v>
+        <v>50.62751318867323</v>
       </c>
       <c r="D48">
-        <v>60.89725693518799</v>
+        <v>60.89725693519265</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1210,13 +1210,13 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>92.25452429212166</v>
+        <v>92.25452429292844</v>
       </c>
       <c r="C49">
-        <v>82.97630886071455</v>
+        <v>82.97630886154334</v>
       </c>
       <c r="D49">
-        <v>81.78421081768064</v>
+        <v>81.78421081842907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>